<commit_message>
excel was added with more numbers
</commit_message>
<xml_diff>
--- a/Exl.xlsx
+++ b/Exl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitZone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F171BE-6E24-43E4-A731-0F5A67374553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66181E50-C5F6-4BDA-8D74-38013E811E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,10 +337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -360,6 +360,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>